<commit_message>
for dietmar: comparison annotations in vcf, gff downloadable from genebank, refseq fasta in ncbi html and PROOKA output
</commit_message>
<xml_diff>
--- a/genom_annot_comp.xlsx
+++ b/genom_annot_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiavasallovega/repolab/work/virusbeacon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F6096D0-9649-9944-917F-E3A0F4DD6719}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C53A5B-2823-7944-BF0C-3B8E8DE1D517}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{87A832D9-CDDA-1644-8535-2A602CE059B1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="158">
   <si>
     <t>proteins in ncbi REFSEQ  html</t>
   </si>
@@ -183,9 +183,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>ORF1ab ppt</t>
-  </si>
-  <si>
     <t>pp1a</t>
   </si>
   <si>
@@ -490,6 +487,18 @@
   </si>
   <si>
     <t>2 utr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>ORF1a (pp1a)</t>
+  </si>
+  <si>
+    <t>ORF1ab (pp1ab)</t>
+  </si>
+  <si>
+    <t>and not really a referrence, but similarity to uniprot of related virus is referenced</t>
   </si>
 </sst>
 </file>
@@ -911,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB5B1E1-94FF-8242-A987-CAA2B66F4149}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>0</v>
@@ -942,28 +951,28 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" t="s">
         <v>57</v>
       </c>
-      <c r="K2" t="s">
-        <v>58</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>52</v>
+        <v>156</v>
       </c>
       <c r="N2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>11</v>
@@ -971,32 +980,32 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>101</v>
+      <c r="A3" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="B3">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="N3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>13</v>
@@ -1006,32 +1015,32 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>107</v>
+      <c r="A4" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="B4">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" t="s">
         <v>136</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" t="s">
-        <v>137</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="N4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>14</v>
@@ -1042,28 +1051,28 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" t="s">
         <v>118</v>
       </c>
-      <c r="F5" t="s">
-        <v>119</v>
-      </c>
       <c r="J5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q5" s="5" t="s">
         <v>15</v>
@@ -1074,22 +1083,22 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>51</v>
@@ -1109,19 +1118,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" t="s">
         <v>122</v>
       </c>
-      <c r="F7" t="s">
-        <v>123</v>
-      </c>
       <c r="J7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="5" t="s">
         <v>17</v>
@@ -1132,7 +1141,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -1141,19 +1150,19 @@
         <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>18</v>
@@ -1164,7 +1173,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1173,17 +1182,17 @@
         <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="2"/>
       <c r="J9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q9" s="5" t="s">
         <v>19</v>
@@ -1194,7 +1203,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1203,13 +1212,13 @@
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q10" s="5" t="s">
         <v>20</v>
@@ -1229,13 +1238,13 @@
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>21</v>
@@ -1246,22 +1255,25 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="Q12" s="5" t="s">
         <v>22</v>
@@ -1272,22 +1284,22 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q13" s="5" t="s">
         <v>23</v>
@@ -1298,19 +1310,19 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q14" s="5" t="s">
         <v>24</v>
@@ -1327,16 +1339,16 @@
         <v>0</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q15" s="5" t="s">
         <v>25</v>
@@ -1347,19 +1359,19 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q16" s="5" t="s">
         <v>26</v>
@@ -1370,19 +1382,19 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q17" s="5" t="s">
         <v>27</v>
@@ -1393,16 +1405,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>28</v>
@@ -1413,16 +1425,16 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I19" t="s">
         <v>43</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>41</v>
@@ -1436,19 +1448,19 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>4</v>
@@ -1459,13 +1471,13 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>5</v>
@@ -1476,16 +1488,16 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E22" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q22" s="5" t="s">
         <v>9</v>
@@ -1499,10 +1511,10 @@
         <v>47</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q23" s="5" t="s">
         <v>10</v>
@@ -1513,10 +1525,13 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J24" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K24" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="N24" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
@@ -1524,7 +1539,7 @@
         <v>46</v>
       </c>
       <c r="K25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -1532,18 +1547,18 @@
         <v>45</v>
       </c>
       <c r="K26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -1551,18 +1566,18 @@
         <v>49</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J29" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -1570,7 +1585,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J31" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -1578,22 +1593,22 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="J32" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J33" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>